<commit_message>
[Err] Missing One Communication Overlap Box
</commit_message>
<xml_diff>
--- a/PingPongSwapDual.csv.xlsx
+++ b/PingPongSwapDual.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhentaofan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC03CDF-6E8F-6645-AFBC-0EEA9B55D4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66726DE0-8B53-5F4F-A10D-68A4697910B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="94" xr2:uid="{5324F66E-2139-471C-8B81-09AA638634E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="76">
   <si>
     <t>x</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>require Layer 1,2,3,4</t>
+  </si>
+  <si>
+    <t>First 8 microbatches</t>
   </si>
 </sst>
 </file>
@@ -3671,13 +3674,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>59</xdr:col>
+      <xdr:col>57</xdr:col>
       <xdr:colOff>345909</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>148635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>60</xdr:col>
+      <xdr:col>58</xdr:col>
       <xdr:colOff>347678</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>151998</xdr:rowOff>
@@ -3727,13 +3730,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>59</xdr:col>
+      <xdr:col>57</xdr:col>
       <xdr:colOff>312511</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>126666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>59</xdr:col>
+      <xdr:col>57</xdr:col>
       <xdr:colOff>312850</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>148338</xdr:rowOff>
@@ -3783,13 +3786,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>58</xdr:col>
+      <xdr:col>56</xdr:col>
       <xdr:colOff>321846</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>167351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>59</xdr:col>
+      <xdr:col>57</xdr:col>
       <xdr:colOff>323615</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>170380</xdr:rowOff>
@@ -3839,13 +3842,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>58</xdr:col>
+      <xdr:col>56</xdr:col>
       <xdr:colOff>347268</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>118311</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>58</xdr:col>
+      <xdr:col>56</xdr:col>
       <xdr:colOff>347607</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>139982</xdr:rowOff>
@@ -3895,13 +3898,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>57</xdr:col>
+      <xdr:col>55</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>185731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>58</xdr:col>
+      <xdr:col>56</xdr:col>
       <xdr:colOff>325620</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>188760</xdr:rowOff>
@@ -3951,13 +3954,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>57</xdr:col>
+      <xdr:col>55</xdr:col>
       <xdr:colOff>345933</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>57</xdr:col>
+      <xdr:col>55</xdr:col>
       <xdr:colOff>346272</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>155021</xdr:rowOff>
@@ -4007,13 +4010,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>60</xdr:col>
+      <xdr:col>58</xdr:col>
       <xdr:colOff>387943</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>123415</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>60</xdr:col>
+      <xdr:col>58</xdr:col>
       <xdr:colOff>388282</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>145420</xdr:rowOff>
@@ -4063,13 +4066,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>177711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>27170</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>180740</xdr:rowOff>
@@ -4119,13 +4122,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>392387</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>129005</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>392726</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>150677</xdr:rowOff>
@@ -4175,13 +4178,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>47458</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>189408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>49228</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>1937</xdr:rowOff>
@@ -4231,13 +4234,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>20745</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>140703</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>21084</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>162374</xdr:rowOff>
@@ -4287,13 +4290,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>62832</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>10605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>64601</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>13634</xdr:rowOff>
@@ -4343,13 +4346,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>35450</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>35789</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>174071</xdr:rowOff>
@@ -4399,13 +4402,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>31300</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>179464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>31639</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>10969</xdr:rowOff>
@@ -4511,13 +4514,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>58</xdr:col>
+      <xdr:col>56</xdr:col>
       <xdr:colOff>35450</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>58</xdr:col>
+      <xdr:col>56</xdr:col>
       <xdr:colOff>35789</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>174071</xdr:rowOff>
@@ -4867,8 +4870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFAD23B-D105-4614-8301-DFD7B66ACD8E}">
   <dimension ref="A1:FE149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="62" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J90" sqref="J90:J91"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AP97" sqref="AP97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12607,6 +12610,9 @@
       <c r="DT66" s="2"/>
     </row>
     <row r="67" spans="4:161" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>75</v>
+      </c>
       <c r="BH67" t="s">
         <v>56</v>
       </c>
@@ -12804,13 +12810,13 @@
       <c r="BL68" s="18">
         <v>1</v>
       </c>
-      <c r="BM68" s="7" t="s">
+      <c r="BM68" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="BN68" s="7" t="s">
+      <c r="BN68" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="BO68" s="29">
+      <c r="BO68" s="32">
         <v>2</v>
       </c>
       <c r="BP68" s="33" t="s">
@@ -13986,13 +13992,13 @@
       <c r="M71" s="18">
         <v>1</v>
       </c>
-      <c r="N71" s="7" t="s">
+      <c r="N71" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="O71" s="7" t="s">
+      <c r="O71" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="P71" s="29">
+      <c r="P71" s="32">
         <v>2</v>
       </c>
       <c r="Q71" s="33" t="s">
@@ -14274,13 +14280,13 @@
       <c r="DK71" s="18">
         <v>1</v>
       </c>
-      <c r="DL71" s="7" t="s">
+      <c r="DL71" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="DM71" s="7" t="s">
+      <c r="DM71" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="DN71" s="29">
+      <c r="DN71" s="32">
         <v>2</v>
       </c>
       <c r="DO71" s="33" t="s">
@@ -14538,10 +14544,12 @@
     <row r="80" spans="4:161" x14ac:dyDescent="0.2">
       <c r="R80" s="1"/>
     </row>
-    <row r="82" spans="6:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F82" s="1" t="s">
+    <row r="82" spans="4:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AE82" s="2"/>
+      <c r="AF82" s="2"/>
       <c r="AG82" s="2"/>
       <c r="AH82" s="2"/>
       <c r="AI82" s="2"/>
@@ -14566,353 +14574,351 @@
       <c r="BB82" s="2"/>
       <c r="BC82" s="2"/>
       <c r="BD82" s="2"/>
-      <c r="BE82" s="2"/>
+      <c r="BE82" t="s">
+        <v>56</v>
+      </c>
       <c r="BF82" s="2"/>
-      <c r="BG82" t="s">
-        <v>56</v>
-      </c>
+      <c r="BG82" s="2"/>
       <c r="BH82" s="2"/>
-      <c r="BI82" s="2"/>
-      <c r="BJ82" s="2"/>
       <c r="BK82" s="2"/>
     </row>
-    <row r="83" spans="6:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="F83" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G83" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H83" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I83" s="20">
+        <v>1</v>
+      </c>
+      <c r="J83" s="20">
+        <v>2</v>
+      </c>
+      <c r="K83" s="20">
+        <v>3</v>
+      </c>
+      <c r="L83" s="20">
+        <v>4</v>
+      </c>
+      <c r="M83" s="18">
+        <v>1</v>
+      </c>
+      <c r="N83" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="O83" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="P83" s="32">
+        <v>2</v>
+      </c>
+      <c r="Q83" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R83" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="S83" s="32">
+        <v>3</v>
+      </c>
+      <c r="T83" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="U83" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="V83" s="32">
+        <v>4</v>
+      </c>
+      <c r="W83" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="X83" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y83" s="35">
+        <v>5</v>
+      </c>
+      <c r="Z83" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA83" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB83" s="34">
+        <v>6</v>
+      </c>
+      <c r="AC83" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD83" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE83" s="34">
+        <v>7</v>
+      </c>
+      <c r="AF83" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG83" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH83" s="34">
+        <v>8</v>
+      </c>
+      <c r="AI83" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ83" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK83" s="32">
+        <v>5</v>
+      </c>
+      <c r="AL83" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM83" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN83" s="32">
+        <v>6</v>
+      </c>
+      <c r="AO83" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP83" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G83" s="22" t="s">
+      <c r="AQ83" s="32">
+        <v>7</v>
+      </c>
+      <c r="AR83" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H83" s="22" t="s">
+      <c r="AS83" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="I83" s="22" t="s">
+      <c r="AT83" s="32">
+        <v>8</v>
+      </c>
+      <c r="AU83" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J83" s="22" t="s">
+      <c r="AV83" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K83" s="20">
-        <v>1</v>
-      </c>
-      <c r="L83" s="20">
+      <c r="AW83" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX83" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY83" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ83" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA83" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB83" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC83" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD83" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE83" s="20">
+        <v>1</v>
+      </c>
+      <c r="BF83" s="20">
         <v>2</v>
       </c>
-      <c r="M83" s="20">
+      <c r="BG83" s="20">
         <v>3</v>
       </c>
-      <c r="N83" s="20">
+      <c r="BH83" s="20">
         <v>4</v>
       </c>
-      <c r="O83" s="18">
-        <v>1</v>
-      </c>
-      <c r="P83" s="7" t="s">
+    </row>
+    <row r="84" spans="4:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D84" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F84" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G84" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H84" s="20">
+        <v>1</v>
+      </c>
+      <c r="I84" s="20">
+        <v>2</v>
+      </c>
+      <c r="J84" s="20">
+        <v>3</v>
+      </c>
+      <c r="K84" s="20">
+        <v>4</v>
+      </c>
+      <c r="L84" s="18">
+        <v>1</v>
+      </c>
+      <c r="M84" s="18">
+        <v>2</v>
+      </c>
+      <c r="P84" s="29">
+        <v>3</v>
+      </c>
+      <c r="Q84" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="Q83" s="7" t="s">
+      <c r="R84" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="R83" s="29">
+      <c r="S84" s="32">
+        <v>4</v>
+      </c>
+      <c r="T84" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="U84" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="V84" s="34">
+        <v>5</v>
+      </c>
+      <c r="W84" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="X84" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y84" s="35">
+        <v>6</v>
+      </c>
+      <c r="Z84" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA84" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB84" s="34">
+        <v>7</v>
+      </c>
+      <c r="AC84" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD84" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE84" s="34">
+        <v>8</v>
+      </c>
+      <c r="AF84" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG84" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH84" s="32">
+        <v>5</v>
+      </c>
+      <c r="AI84" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ84" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK84" s="32">
+        <v>6</v>
+      </c>
+      <c r="AL84" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM84" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN84" s="32">
+        <v>7</v>
+      </c>
+      <c r="AO84" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP84" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ84" s="32">
+        <v>8</v>
+      </c>
+      <c r="AR84" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS84" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT84" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU84" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV84" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW84" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX84" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY84" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AZ84" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA84" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB84" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC84" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD84" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE84" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="BF84" s="20">
+        <v>1</v>
+      </c>
+      <c r="BG84" s="20">
         <v>2</v>
       </c>
-      <c r="S83" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="T83" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="U83" s="32">
-        <v>3</v>
-      </c>
-      <c r="V83" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="W83" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="X83" s="32">
-        <v>4</v>
-      </c>
-      <c r="Y83" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z83" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA83" s="35">
-        <v>5</v>
-      </c>
-      <c r="AB83" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC83" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD83" s="34">
-        <v>6</v>
-      </c>
-      <c r="AE83" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF83" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG83" s="34">
-        <v>7</v>
-      </c>
-      <c r="AH83" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI83" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ83" s="34">
-        <v>8</v>
-      </c>
-      <c r="AK83" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL83" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM83" s="32">
-        <v>5</v>
-      </c>
-      <c r="AN83" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="AO83" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP83" s="32">
-        <v>6</v>
-      </c>
-      <c r="AQ83" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR83" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS83" s="32">
-        <v>7</v>
-      </c>
-      <c r="AT83" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="AU83" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV83" s="32">
-        <v>8</v>
-      </c>
-      <c r="AW83" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX83" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="AY83" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="AZ83" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="BA83" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB83" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="BC83" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="BD83" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="BE83" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF83" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="BG83" s="20">
-        <v>1</v>
-      </c>
-      <c r="BH83" s="20">
-        <v>2</v>
-      </c>
-      <c r="BI83" s="20">
-        <v>3</v>
-      </c>
-      <c r="BJ83" s="20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="6:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F84" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G84" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H84" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="I84" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="J84" s="20">
-        <v>1</v>
-      </c>
-      <c r="K84" s="20">
-        <v>2</v>
-      </c>
-      <c r="L84" s="20">
-        <v>3</v>
-      </c>
-      <c r="M84" s="20">
-        <v>4</v>
-      </c>
-      <c r="N84" s="18">
-        <v>1</v>
-      </c>
-      <c r="O84" s="18">
-        <v>2</v>
-      </c>
-      <c r="R84" s="29">
-        <v>3</v>
-      </c>
-      <c r="S84" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="T84" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="U84" s="32">
-        <v>4</v>
-      </c>
-      <c r="V84" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="W84" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="X84" s="34">
-        <v>5</v>
-      </c>
-      <c r="Y84" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z84" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA84" s="35">
-        <v>6</v>
-      </c>
-      <c r="AB84" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC84" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD84" s="34">
-        <v>7</v>
-      </c>
-      <c r="AE84" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF84" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG84" s="34">
-        <v>8</v>
-      </c>
-      <c r="AH84" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI84" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ84" s="32">
-        <v>5</v>
-      </c>
-      <c r="AK84" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL84" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM84" s="32">
-        <v>6</v>
-      </c>
-      <c r="AN84" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO84" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP84" s="32">
-        <v>7</v>
-      </c>
-      <c r="AQ84" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="AR84" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="AS84" s="32">
-        <v>8</v>
-      </c>
-      <c r="AT84" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU84" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AV84" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="AW84" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="AX84" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY84" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ84" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="BA84" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="BB84" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC84" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD84" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE84" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="BF84" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG84" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="BH84" s="20">
-        <v>1</v>
-      </c>
-      <c r="BI84" s="20">
-        <v>2</v>
-      </c>
-      <c r="BJ84" s="20">
         <v>3</v>
       </c>
       <c r="BL84" s="2"/>
@@ -14942,359 +14948,359 @@
       <c r="CJ84" s="2"/>
       <c r="CK84" s="2"/>
     </row>
-    <row r="85" spans="6:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="F85" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G85" s="20">
+        <v>1</v>
+      </c>
+      <c r="H85" s="20">
+        <v>2</v>
+      </c>
+      <c r="I85" s="20">
+        <v>3</v>
+      </c>
+      <c r="J85" s="20">
+        <v>4</v>
+      </c>
+      <c r="K85" s="18">
+        <v>1</v>
+      </c>
+      <c r="L85" s="18">
+        <v>2</v>
+      </c>
+      <c r="M85" s="18">
+        <v>3</v>
+      </c>
+      <c r="N85" s="18">
+        <v>4</v>
+      </c>
+      <c r="S85" s="30">
+        <v>5</v>
+      </c>
+      <c r="T85" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="U85" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="V85" s="34">
+        <v>6</v>
+      </c>
+      <c r="W85" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="X85" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y85" s="35">
+        <v>7</v>
+      </c>
+      <c r="Z85" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA85" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB85" s="34">
+        <v>8</v>
+      </c>
+      <c r="AC85" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD85" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE85" s="32">
+        <v>5</v>
+      </c>
+      <c r="AF85" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG85" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH85" s="32">
+        <v>6</v>
+      </c>
+      <c r="AI85" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ85" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK85" s="32">
+        <v>7</v>
+      </c>
+      <c r="AL85" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM85" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN85" s="32">
+        <v>8</v>
+      </c>
+      <c r="AO85" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP85" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ85" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AR85" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS85" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT85" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU85" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV85" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G85" s="22" t="s">
+      <c r="AW85" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H85" s="22" t="s">
+      <c r="AX85" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I85" s="20">
-        <v>1</v>
-      </c>
-      <c r="J85" s="20">
+      <c r="AY85" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AZ85" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="BA85" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB85" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC85" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD85" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE85" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF85" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="BG85" s="20">
+        <v>1</v>
+      </c>
+      <c r="BH85" s="20">
         <v>2</v>
       </c>
-      <c r="K85" s="20">
+    </row>
+    <row r="86" spans="4:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E86" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F86" s="20">
+        <v>1</v>
+      </c>
+      <c r="G86" s="20">
+        <v>2</v>
+      </c>
+      <c r="H86" s="20">
         <v>3</v>
       </c>
-      <c r="L85" s="20">
+      <c r="I86" s="20">
         <v>4</v>
       </c>
-      <c r="M85" s="18">
-        <v>1</v>
-      </c>
-      <c r="N85" s="18">
+      <c r="J86" s="18">
+        <v>1</v>
+      </c>
+      <c r="K86" s="18">
         <v>2</v>
       </c>
-      <c r="O85" s="18">
+      <c r="L86" s="18">
         <v>3</v>
       </c>
-      <c r="P85" s="18">
+      <c r="M86" s="18">
         <v>4</v>
       </c>
-      <c r="U85" s="30">
+      <c r="N86" s="20">
         <v>5</v>
       </c>
-      <c r="V85" s="31" t="s">
+      <c r="O86" s="20">
+        <v>6</v>
+      </c>
+      <c r="V86" s="30">
+        <v>7</v>
+      </c>
+      <c r="W86" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="W85" s="23" t="s">
+      <c r="X86" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="X85" s="34">
+      <c r="Y86" s="35">
+        <v>8</v>
+      </c>
+      <c r="Z86" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA86" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB86" s="32">
+        <v>5</v>
+      </c>
+      <c r="AC86" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD86" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE86" s="32">
         <v>6</v>
       </c>
-      <c r="Y85" s="33" t="s">
+      <c r="AF86" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG86" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH86" s="32">
+        <v>7</v>
+      </c>
+      <c r="AI86" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ86" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK86" s="32">
+        <v>8</v>
+      </c>
+      <c r="AL86" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="Z85" s="24" t="s">
+      <c r="AM86" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AA85" s="35">
-        <v>7</v>
-      </c>
-      <c r="AB85" s="31" t="s">
+      <c r="AN86" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="AC85" s="23" t="s">
+      <c r="AO86" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AD85" s="34">
-        <v>8</v>
-      </c>
-      <c r="AE85" s="33" t="s">
+      <c r="AP86" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AF85" s="24" t="s">
+      <c r="AQ86" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AG85" s="32">
-        <v>5</v>
-      </c>
-      <c r="AH85" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI85" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ85" s="32">
-        <v>6</v>
-      </c>
-      <c r="AK85" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL85" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM85" s="32">
-        <v>7</v>
-      </c>
-      <c r="AN85" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO85" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="AP85" s="32">
-        <v>8</v>
-      </c>
-      <c r="AQ85" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR85" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS85" s="19" t="s">
+      <c r="AR86" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AT85" s="19" t="s">
+      <c r="AS86" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AU85" s="19" t="s">
+      <c r="AT86" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AV85" s="19" t="s">
+      <c r="AU86" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AW85" s="19" t="s">
+      <c r="AV86" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AX85" s="19" t="s">
+      <c r="AW86" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="AY85" s="19" t="s">
+      <c r="AX86" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AZ85" s="19" t="s">
+      <c r="AY86" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="BA85" s="22" t="s">
+      <c r="AZ86" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="BB85" s="22" t="s">
+      <c r="BA86" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="BC85" s="22" t="s">
+      <c r="BB86" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="BD85" s="22" t="s">
+      <c r="BC86" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="BE85" s="22" t="s">
+      <c r="BD86" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="BF85" s="22" t="s">
+      <c r="BE86" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="BG85" s="22" t="s">
+      <c r="BF86" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="BH85" s="22" t="s">
+      <c r="BG86" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="BI85" s="20">
-        <v>1</v>
-      </c>
-      <c r="BJ85" s="20">
-        <v>2</v>
+      <c r="BH86" s="20">
+        <v>1</v>
       </c>
     </row>
-    <row r="86" spans="6:89" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F86" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G86" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="H86" s="20">
-        <v>1</v>
-      </c>
-      <c r="I86" s="20">
-        <v>2</v>
-      </c>
-      <c r="J86" s="20">
-        <v>3</v>
-      </c>
-      <c r="K86" s="20">
-        <v>4</v>
-      </c>
-      <c r="L86" s="18">
-        <v>1</v>
-      </c>
-      <c r="M86" s="18">
-        <v>2</v>
-      </c>
-      <c r="N86" s="18">
-        <v>3</v>
-      </c>
-      <c r="O86" s="18">
-        <v>4</v>
-      </c>
-      <c r="P86" s="20">
-        <v>5</v>
-      </c>
-      <c r="Q86" s="20">
-        <v>6</v>
-      </c>
-      <c r="X86" s="30">
-        <v>7</v>
-      </c>
-      <c r="Y86" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z86" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA86" s="35">
-        <v>8</v>
-      </c>
-      <c r="AB86" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC86" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD86" s="32">
-        <v>5</v>
-      </c>
-      <c r="AE86" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF86" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG86" s="32">
-        <v>6</v>
-      </c>
-      <c r="AH86" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI86" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ86" s="32">
-        <v>7</v>
-      </c>
-      <c r="AK86" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL86" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM86" s="32">
-        <v>8</v>
-      </c>
-      <c r="AN86" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AO86" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AP86" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="AQ86" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="AR86" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS86" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT86" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="AU86" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="AV86" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW86" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AX86" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY86" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="AZ86" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA86" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="BB86" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="BC86" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="BD86" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="BE86" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="BF86" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="BG86" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="BH86" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI86" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="BJ86" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX87" s="2"/>
       <c r="AY87" s="2"/>
       <c r="AZ87" s="2"/>
       <c r="BA87" s="2"/>
     </row>
-    <row r="88" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX88" s="2"/>
       <c r="AY88" s="2"/>
       <c r="AZ88" s="2"/>
       <c r="BA88" s="2"/>
     </row>
-    <row r="89" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX89" s="2"/>
       <c r="AY89" s="2"/>
       <c r="AZ89" s="2"/>
       <c r="BA89" s="2"/>
     </row>
-    <row r="92" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX92" s="2"/>
       <c r="AY92" s="2"/>
       <c r="AZ92" s="2"/>
       <c r="BA92" s="2"/>
     </row>
-    <row r="93" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX93" s="2"/>
       <c r="AY93" s="2"/>
       <c r="AZ93" s="2"/>
       <c r="BA93" s="2"/>
     </row>
-    <row r="94" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX94" s="2"/>
       <c r="AY94" s="2"/>
       <c r="AZ94" s="2"/>
       <c r="BA94" s="2"/>
     </row>
-    <row r="95" spans="6:89" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:89" x14ac:dyDescent="0.2">
       <c r="AX95" s="2"/>
       <c r="AY95" s="2"/>
       <c r="AZ95" s="2"/>

</xml_diff>